<commit_message>
Fix difference in hand count
</commit_message>
<xml_diff>
--- a/Differences in Hand Counts.xlsx
+++ b/Differences in Hand Counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19099\Documents\Kaul_Lab\AutoCellCount\Automatic-Cell-counting-with-TWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB3F008-7F54-4620-8600-3E8D1BFBE521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575A7730-3E75-4932-AF8B-59F97031FA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8928" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1146,7 +1146,7 @@
   <dimension ref="A1:D264"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D264"/>
+      <selection activeCell="B2" sqref="B2:B264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4564,7 +4564,7 @@
         <v>245</v>
       </c>
       <c r="B244">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C244">
         <v>111</v>
@@ -4578,7 +4578,7 @@
         <v>246</v>
       </c>
       <c r="B245">
-        <v>175</v>
+        <v>87</v>
       </c>
       <c r="C245">
         <v>87</v>
@@ -4592,7 +4592,7 @@
         <v>247</v>
       </c>
       <c r="B246">
-        <v>176</v>
+        <v>91</v>
       </c>
       <c r="C246">
         <v>84</v>
@@ -4606,7 +4606,7 @@
         <v>248</v>
       </c>
       <c r="B247">
-        <v>163</v>
+        <v>80</v>
       </c>
       <c r="C247">
         <v>82</v>
@@ -4620,7 +4620,7 @@
         <v>249</v>
       </c>
       <c r="B248">
-        <v>166</v>
+        <v>87</v>
       </c>
       <c r="C248">
         <v>78</v>
@@ -4634,7 +4634,7 @@
         <v>250</v>
       </c>
       <c r="B249">
-        <v>120</v>
+        <v>58</v>
       </c>
       <c r="C249">
         <v>61</v>
@@ -4648,7 +4648,7 @@
         <v>251</v>
       </c>
       <c r="B250">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="C250">
         <v>57</v>
@@ -4662,7 +4662,7 @@
         <v>252</v>
       </c>
       <c r="B251">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="C251">
         <v>28</v>
@@ -4676,7 +4676,7 @@
         <v>253</v>
       </c>
       <c r="B252">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="C252">
         <v>33</v>
@@ -4690,7 +4690,7 @@
         <v>254</v>
       </c>
       <c r="B253">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="C253">
         <v>54</v>
@@ -4704,7 +4704,7 @@
         <v>255</v>
       </c>
       <c r="B254">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="C254">
         <v>61</v>
@@ -4718,7 +4718,7 @@
         <v>256</v>
       </c>
       <c r="B255">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="C255">
         <v>30</v>
@@ -4732,7 +4732,7 @@
         <v>257</v>
       </c>
       <c r="B256">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="C256">
         <v>54</v>
@@ -4746,7 +4746,7 @@
         <v>258</v>
       </c>
       <c r="B257">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="C257">
         <v>54</v>
@@ -4760,7 +4760,7 @@
         <v>259</v>
       </c>
       <c r="B258">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="C258">
         <v>37</v>
@@ -4774,7 +4774,7 @@
         <v>260</v>
       </c>
       <c r="B259">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="C259">
         <v>27</v>
@@ -4788,7 +4788,7 @@
         <v>261</v>
       </c>
       <c r="B260">
-        <v>72</v>
+        <v>36</v>
       </c>
       <c r="C260">
         <v>35</v>
@@ -4802,7 +4802,7 @@
         <v>262</v>
       </c>
       <c r="B261">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="C261">
         <v>51</v>
@@ -4816,7 +4816,7 @@
         <v>263</v>
       </c>
       <c r="B262">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C262">
         <v>15</v>
@@ -4830,7 +4830,7 @@
         <v>264</v>
       </c>
       <c r="B263">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="C263">
         <v>50</v>
@@ -4844,7 +4844,7 @@
         <v>265</v>
       </c>
       <c r="B264">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C264">
         <v>20</v>

</xml_diff>